<commit_message>
add Iluem site (#540)
</commit_message>
<xml_diff>
--- a/cms/templates/bulk-model-upload.xlsx
+++ b/cms/templates/bulk-model-upload.xlsx
@@ -15,12 +15,12 @@
     <sheet name="Upload" sheetId="1" r:id="rId1"/>
     <sheet name="EnumSheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="504">
   <si>
     <t>Name</t>
   </si>
@@ -1529,6 +1529,9 @@
   </si>
   <si>
     <t>Endometrial cancer</t>
+  </si>
+  <si>
+    <t>Extrahepatic bile duct</t>
   </si>
 </sst>
 </file>
@@ -2418,8 +2421,8 @@
   </sheetPr>
   <dimension ref="A1:AG1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="V32" sqref="V32:V34"/>
+    <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
+      <selection activeCell="M401" sqref="M401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17455,7 +17458,9 @@
       <c r="J401" s="10"/>
       <c r="K401" s="10"/>
       <c r="L401" s="10"/>
-      <c r="M401" s="10"/>
+      <c r="M401" s="15" t="s">
+        <v>503</v>
+      </c>
       <c r="N401" s="10"/>
       <c r="O401" s="10"/>
       <c r="P401" s="10"/>

</xml_diff>